<commit_message>
sn: preatas sept 2021 - update form for phase 3
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Senegal/septembre 2021/sn_lf_pretas_2_partcipants_202109.xlsx
+++ b/LF/PreTAS/Senegal/septembre 2021/sn_lf_pretas_2_partcipants_202109.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Senegal\septembre 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F06713-D29D-49BF-BDB9-B3E1CA7D086C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF173A3E-4864-4A67-AE54-8BCFF2A6E2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13" yWindow="13" windowWidth="25587" windowHeight="13787" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -353,10 +353,10 @@
     <t>L'age doit être compris entre 6 et 120 ans</t>
   </si>
   <si>
-    <t>sn_lf_pretas_2_partcipants_202109</t>
-  </si>
-  <si>
-    <t>(Septembre 2021) 2. Pre-TAS FL Formulaire Participants</t>
+    <t>(Septembre 2021) 2. Pre-TAS FL Formulaire Participants V2</t>
+  </si>
+  <si>
+    <t>sn_lf_pretas_2_partcipants_202109_v2</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1410,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4:B5"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -1533,7 +1533,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -1559,10 +1559,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
         <v>108</v>
-      </c>
-      <c r="B2" t="s">
-        <v>107</v>
       </c>
       <c r="C2">
         <v>20210722</v>

</xml_diff>